<commit_message>
updated a number of components of iran
</commit_message>
<xml_diff>
--- a/iran/transformations/templates/calibrated/iran/model_input_variables_iran_se_calibrated.xlsx
+++ b/iran/transformations/templates/calibrated/iran/model_input_variables_iran_se_calibrated.xlsx
@@ -11,13 +11,14 @@
     <sheet name="strategy_id-6003" sheetId="2" r:id="rId2"/>
     <sheet name="strategy_id-6004" sheetId="3" r:id="rId3"/>
     <sheet name="strategy_id-6005" sheetId="4" r:id="rId4"/>
+    <sheet name="strategy_id-7032" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
   <si>
     <t>subsector</t>
   </si>
@@ -1091,109 +1092,109 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>0.8100000000000001</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>0.79</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="AG6">
-        <v>0.77</v>
+        <v>1</v>
       </c>
       <c r="AH6">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>0.74</v>
+        <v>1</v>
       </c>
       <c r="AK6">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="AL6">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="AM6">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="AN6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AO6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AP6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AQ6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AR6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AS6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -2098,109 +2099,109 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0.9958333333333333</v>
+      </c>
+      <c r="W2">
+        <v>0.9916666666666666</v>
+      </c>
+      <c r="X2">
+        <v>0.9875</v>
+      </c>
+      <c r="Y2">
+        <v>0.9833333333333334</v>
+      </c>
+      <c r="Z2">
+        <v>0.9791666666666666</v>
+      </c>
+      <c r="AA2">
+        <v>0.975</v>
+      </c>
+      <c r="AB2">
+        <v>0.9708333333333332</v>
+      </c>
+      <c r="AC2">
+        <v>0.9666666666666668</v>
+      </c>
+      <c r="AD2">
+        <v>0.9625</v>
+      </c>
+      <c r="AE2">
+        <v>0.9583333333333333</v>
+      </c>
+      <c r="AF2">
+        <v>0.9541666666666667</v>
+      </c>
+      <c r="AG2">
         <v>0.95</v>
       </c>
-      <c r="P2">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="Q2">
-        <v>0.93</v>
-      </c>
-      <c r="R2">
-        <v>0.92</v>
-      </c>
-      <c r="S2">
-        <v>0.91</v>
-      </c>
-      <c r="T2">
+      <c r="AH2">
+        <v>0.9458333333333333</v>
+      </c>
+      <c r="AI2">
+        <v>0.9416666666666667</v>
+      </c>
+      <c r="AJ2">
+        <v>0.9375</v>
+      </c>
+      <c r="AK2">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="AL2">
+        <v>0.9291666666666667</v>
+      </c>
+      <c r="AM2">
+        <v>0.925</v>
+      </c>
+      <c r="AN2">
+        <v>0.9208333333333334</v>
+      </c>
+      <c r="AO2">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="AP2">
+        <v>0.9125</v>
+      </c>
+      <c r="AQ2">
+        <v>0.9083333333333333</v>
+      </c>
+      <c r="AR2">
+        <v>0.9041666666666667</v>
+      </c>
+      <c r="AS2">
         <v>0.9</v>
-      </c>
-      <c r="U2">
-        <v>0.89</v>
-      </c>
-      <c r="V2">
-        <v>0.8475</v>
-      </c>
-      <c r="W2">
-        <v>0.8058333333333333</v>
-      </c>
-      <c r="X2">
-        <v>0.7649999999999999</v>
-      </c>
-      <c r="Y2">
-        <v>0.7250000000000001</v>
-      </c>
-      <c r="Z2">
-        <v>0.6858333333333333</v>
-      </c>
-      <c r="AA2">
-        <v>0.6475</v>
-      </c>
-      <c r="AB2">
-        <v>0.6099999999999999</v>
-      </c>
-      <c r="AC2">
-        <v>0.5733333333333335</v>
-      </c>
-      <c r="AD2">
-        <v>0.5375</v>
-      </c>
-      <c r="AE2">
-        <v>0.5024999999999999</v>
-      </c>
-      <c r="AF2">
-        <v>0.4683333333333334</v>
-      </c>
-      <c r="AG2">
-        <v>0.435</v>
-      </c>
-      <c r="AH2">
-        <v>0.4025000000000001</v>
-      </c>
-      <c r="AI2">
-        <v>0.3708333333333333</v>
-      </c>
-      <c r="AJ2">
-        <v>0.34</v>
-      </c>
-      <c r="AK2">
-        <v>0.31</v>
-      </c>
-      <c r="AL2">
-        <v>0.2808333333333333</v>
-      </c>
-      <c r="AM2">
-        <v>0.2525</v>
-      </c>
-      <c r="AN2">
-        <v>0.225</v>
-      </c>
-      <c r="AO2">
-        <v>0.2</v>
-      </c>
-      <c r="AP2">
-        <v>0.175</v>
-      </c>
-      <c r="AQ2">
-        <v>0.15</v>
-      </c>
-      <c r="AR2">
-        <v>0.125</v>
-      </c>
-      <c r="AS2">
-        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -2373,109 +2374,109 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0.9875</v>
+      </c>
+      <c r="W2">
+        <v>0.975</v>
+      </c>
+      <c r="X2">
+        <v>0.9625</v>
+      </c>
+      <c r="Y2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="Z2">
+        <v>0.9375</v>
+      </c>
+      <c r="AA2">
+        <v>0.925</v>
+      </c>
+      <c r="AB2">
+        <v>0.9124999999999999</v>
+      </c>
+      <c r="AC2">
         <v>0.9</v>
       </c>
-      <c r="U2">
-        <v>0.89</v>
-      </c>
-      <c r="V2">
-        <v>0.8558333333333333</v>
-      </c>
-      <c r="W2">
-        <v>0.8225</v>
-      </c>
-      <c r="X2">
-        <v>0.7899999999999999</v>
-      </c>
-      <c r="Y2">
-        <v>0.7583333333333334</v>
-      </c>
-      <c r="Z2">
-        <v>0.7274999999999999</v>
-      </c>
-      <c r="AA2">
-        <v>0.6974999999999999</v>
-      </c>
-      <c r="AB2">
-        <v>0.6683333333333332</v>
-      </c>
-      <c r="AC2">
-        <v>0.6400000000000001</v>
-      </c>
       <c r="AD2">
-        <v>0.6125</v>
+        <v>0.8875</v>
       </c>
       <c r="AE2">
-        <v>0.5858333333333333</v>
+        <v>0.875</v>
       </c>
       <c r="AF2">
-        <v>0.5600000000000001</v>
+        <v>0.8625</v>
       </c>
       <c r="AG2">
-        <v>0.535</v>
+        <v>0.85</v>
       </c>
       <c r="AH2">
-        <v>0.5108333333333334</v>
+        <v>0.8374999999999999</v>
       </c>
       <c r="AI2">
-        <v>0.4875</v>
+        <v>0.825</v>
       </c>
       <c r="AJ2">
-        <v>0.465</v>
+        <v>0.8125</v>
       </c>
       <c r="AK2">
-        <v>0.4433333333333334</v>
+        <v>0.8</v>
       </c>
       <c r="AL2">
-        <v>0.4225</v>
+        <v>0.7875</v>
       </c>
       <c r="AM2">
-        <v>0.4025</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AN2">
-        <v>0.3833333333333333</v>
+        <v>0.7625</v>
       </c>
       <c r="AO2">
-        <v>0.3666666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="AP2">
-        <v>0.35</v>
+        <v>0.7374999999999999</v>
       </c>
       <c r="AQ2">
-        <v>0.3333333333333333</v>
+        <v>0.725</v>
       </c>
       <c r="AR2">
-        <v>0.3166666666666666</v>
+        <v>0.7124999999999999</v>
       </c>
       <c r="AS2">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -2648,109 +2649,384 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0.9875</v>
+      </c>
+      <c r="W2">
+        <v>0.975</v>
+      </c>
+      <c r="X2">
+        <v>0.9625</v>
+      </c>
+      <c r="Y2">
+        <v>0.9500000000000001</v>
+      </c>
+      <c r="Z2">
+        <v>0.9375</v>
+      </c>
+      <c r="AA2">
+        <v>0.925</v>
+      </c>
+      <c r="AB2">
+        <v>0.9124999999999999</v>
+      </c>
+      <c r="AC2">
         <v>0.9</v>
       </c>
+      <c r="AD2">
+        <v>0.8875</v>
+      </c>
+      <c r="AE2">
+        <v>0.875</v>
+      </c>
+      <c r="AF2">
+        <v>0.8625</v>
+      </c>
+      <c r="AG2">
+        <v>0.85</v>
+      </c>
+      <c r="AH2">
+        <v>0.8374999999999999</v>
+      </c>
+      <c r="AI2">
+        <v>0.825</v>
+      </c>
+      <c r="AJ2">
+        <v>0.8125</v>
+      </c>
+      <c r="AK2">
+        <v>0.8</v>
+      </c>
+      <c r="AL2">
+        <v>0.7875</v>
+      </c>
+      <c r="AM2">
+        <v>0.7749999999999999</v>
+      </c>
+      <c r="AN2">
+        <v>0.7625</v>
+      </c>
+      <c r="AO2">
+        <v>0.75</v>
+      </c>
+      <c r="AP2">
+        <v>0.7374999999999999</v>
+      </c>
+      <c r="AQ2">
+        <v>0.725</v>
+      </c>
+      <c r="AR2">
+        <v>0.7124999999999999</v>
+      </c>
+      <c r="AS2">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
       <c r="U2">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>0.8558333333333333</v>
+        <v>0.9875</v>
       </c>
       <c r="W2">
-        <v>0.8225</v>
+        <v>0.975</v>
       </c>
       <c r="X2">
-        <v>0.7899999999999999</v>
+        <v>0.9625</v>
       </c>
       <c r="Y2">
-        <v>0.7583333333333334</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="Z2">
-        <v>0.7274999999999999</v>
+        <v>0.9375</v>
       </c>
       <c r="AA2">
-        <v>0.6974999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB2">
-        <v>0.6683333333333332</v>
+        <v>0.9124999999999999</v>
       </c>
       <c r="AC2">
-        <v>0.6400000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AD2">
-        <v>0.6125</v>
+        <v>0.8875</v>
       </c>
       <c r="AE2">
-        <v>0.5858333333333333</v>
+        <v>0.875</v>
       </c>
       <c r="AF2">
-        <v>0.5600000000000001</v>
+        <v>0.8625</v>
       </c>
       <c r="AG2">
-        <v>0.535</v>
+        <v>0.85</v>
       </c>
       <c r="AH2">
-        <v>0.5108333333333334</v>
+        <v>0.8374999999999999</v>
       </c>
       <c r="AI2">
-        <v>0.4875</v>
+        <v>0.825</v>
       </c>
       <c r="AJ2">
-        <v>0.465</v>
+        <v>0.8125</v>
       </c>
       <c r="AK2">
-        <v>0.4433333333333334</v>
+        <v>0.8</v>
       </c>
       <c r="AL2">
-        <v>0.4225</v>
+        <v>0.7875</v>
       </c>
       <c r="AM2">
-        <v>0.4025</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AN2">
-        <v>0.3833333333333333</v>
+        <v>0.7625</v>
       </c>
       <c r="AO2">
-        <v>0.3666666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="AP2">
-        <v>0.35</v>
+        <v>0.7374999999999999</v>
       </c>
       <c r="AQ2">
-        <v>0.3333333333333333</v>
+        <v>0.725</v>
       </c>
       <c r="AR2">
-        <v>0.3166666666666666</v>
+        <v>0.7124999999999999</v>
       </c>
       <c r="AS2">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating iran before modifyin strategy_definitions
</commit_message>
<xml_diff>
--- a/iran/transformations/templates/calibrated/iran/model_input_variables_iran_se_calibrated.xlsx
+++ b/iran/transformations/templates/calibrated/iran/model_input_variables_iran_se_calibrated.xlsx
@@ -11,14 +11,13 @@
     <sheet name="strategy_id-6003" sheetId="2" r:id="rId2"/>
     <sheet name="strategy_id-6004" sheetId="3" r:id="rId3"/>
     <sheet name="strategy_id-6005" sheetId="4" r:id="rId4"/>
-    <sheet name="strategy_id-7032" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
   <si>
     <t>subsector</t>
   </si>
@@ -2757,279 +2756,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>0.9875</v>
-      </c>
-      <c r="W2">
-        <v>0.975</v>
-      </c>
-      <c r="X2">
-        <v>0.9625</v>
-      </c>
-      <c r="Y2">
-        <v>0.9500000000000001</v>
-      </c>
-      <c r="Z2">
-        <v>0.9375</v>
-      </c>
-      <c r="AA2">
-        <v>0.925</v>
-      </c>
-      <c r="AB2">
-        <v>0.9124999999999999</v>
-      </c>
-      <c r="AC2">
-        <v>0.9</v>
-      </c>
-      <c r="AD2">
-        <v>0.8875</v>
-      </c>
-      <c r="AE2">
-        <v>0.875</v>
-      </c>
-      <c r="AF2">
-        <v>0.8625</v>
-      </c>
-      <c r="AG2">
-        <v>0.85</v>
-      </c>
-      <c r="AH2">
-        <v>0.8374999999999999</v>
-      </c>
-      <c r="AI2">
-        <v>0.825</v>
-      </c>
-      <c r="AJ2">
-        <v>0.8125</v>
-      </c>
-      <c r="AK2">
-        <v>0.8</v>
-      </c>
-      <c r="AL2">
-        <v>0.7875</v>
-      </c>
-      <c r="AM2">
-        <v>0.7749999999999999</v>
-      </c>
-      <c r="AN2">
-        <v>0.7625</v>
-      </c>
-      <c r="AO2">
-        <v>0.75</v>
-      </c>
-      <c r="AP2">
-        <v>0.7374999999999999</v>
-      </c>
-      <c r="AQ2">
-        <v>0.725</v>
-      </c>
-      <c r="AR2">
-        <v>0.7124999999999999</v>
-      </c>
-      <c r="AS2">
-        <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>